<commit_message>
Fix errors according to comments
</commit_message>
<xml_diff>
--- a/Exc2/FURPS.xlsx
+++ b/Exc2/FURPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1234/src/yandex/sprint_9/architecture-sprint-9/Exc2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E0B51F-60FD-8F49-8358-DB0A3017144C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97709BF-60BE-8845-8B85-FF9AAF92206E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-10300" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-10300" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Код</t>
   </si>
@@ -188,6 +188,63 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>Клиент может подать заявку на открытие депозита</t>
+  </si>
+  <si>
+    <t>Менеджер по депозитным процессам обрабатывает заявки в бек-офисе, подтверждая условия депозита в АБС банка</t>
+  </si>
+  <si>
+    <t>Сотрудник отделения может подать заявку напрямую в АБС, если клиент сразу придет в отделение, чтобы открыть депозит</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>Отклик интерфейса должен занимать миллисекунды</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Документация по системе</t>
+  </si>
+  <si>
+    <t>Нужно использовать микросервисную архитектуру при разработке в интернет-банке</t>
+  </si>
+  <si>
+    <t>АБС поддерживает только вертикальное масштабирование</t>
+  </si>
+  <si>
+    <t>Использовать Kafka для очередей сообщений</t>
+  </si>
+  <si>
+    <t>Использовать платформы Java, .NET, PHP</t>
+  </si>
+  <si>
+    <t>Использовать существующие базы данных Oracle, MS SQL</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
   </si>
 </sst>
 </file>
@@ -335,20 +392,20 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,17 +634,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="168" zoomScaleNormal="214" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="168" zoomScaleNormal="214" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.3984375" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="6.83203125" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.796875" customWidth="1"/>
+    <col min="3" max="3" width="35.796875" customWidth="1"/>
+    <col min="4" max="4" width="44.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="30" customHeight="1"/>
@@ -607,16 +664,16 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:4" ht="30" customHeight="1">
       <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="4"/>
@@ -636,198 +693,293 @@
       <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="2:4" ht="30" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="2:4" ht="30" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30" customHeight="1">
+    <row r="10" spans="2:4" ht="28">
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="2:4" ht="30" customHeight="1">
-      <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:4" ht="30" customHeight="1">
+    <row r="11" spans="2:4" ht="56">
+      <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="2:4" ht="56">
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:4" ht="30" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="2:4" ht="30" customHeight="1">
       <c r="B14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="2:4" ht="30" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="2:4" ht="30" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>32</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13"/>
     </row>
     <row r="17" spans="1:4" ht="30" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="10"/>
+        <v>45</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1">
       <c r="B18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1">
       <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1">
       <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1">
       <c r="B21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>35</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1">
       <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1">
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" customHeight="1">
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" customHeight="1">
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" customHeight="1">
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="10"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" customHeight="1">
+      <c r="B27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C27" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5" t="s">
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A28" s="8"/>
+      <c r="B28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="35.25" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5" t="s">
+    <row r="29" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A29" s="8"/>
+      <c r="B29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" ht="33" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5" t="s">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A31" s="8"/>
+      <c r="B31" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="35.25" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="68">
+      <c r="A34" s="8"/>
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="33" customHeight="1">
+      <c r="A35" s="8"/>
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>

</xml_diff>